<commit_message>
Add method of adding lab member
</commit_message>
<xml_diff>
--- a/excel/PeopleEquipment.xlsx
+++ b/excel/PeopleEquipment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">itemID</t>
   </si>
@@ -28,34 +28,22 @@
     <t xml:space="preserve">label</t>
   </si>
   <si>
-    <t xml:space="preserve">aaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a aa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bbb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b bb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ccc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c cc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ddd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d dd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e ee</t>
+    <t xml:space="preserve">sasaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">佐々木一郎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">佐藤二郎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">田中三郎</t>
   </si>
 </sst>
 </file>
@@ -162,10 +150,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -177,7 +165,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="46.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="46.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.59"/>
@@ -226,22 +214,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>